<commit_message>
【imp】add permisison check api for create project
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-iam-menu-user-role-label.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-iam-menu-user-role-label.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\hzero-iam\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A81A4-099E-4AE8-8BFF-30865AB941F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B8AA3B-FE2E-42AB-B311-279B7569B8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5879" uniqueCount="1848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5881" uniqueCount="1850">
   <si>
     <r>
       <rPr>
@@ -7417,12 +7417,18 @@
   <si>
     <t>iam_menu_permission-307</t>
   </si>
+  <si>
+    <t>hzero-iam.choerodon-project-user.check</t>
+  </si>
+  <si>
+    <t>iam_menu_permission-308</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="93">
+  <fonts count="94">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -7992,6 +7998,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -8131,7 +8144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8280,6 +8293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -8628,21 +8642,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.58203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.08203125" customWidth="1"/>
     <col min="4" max="4" width="35.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="38.58203125" customWidth="1"/>
+    <col min="6" max="6" width="23.4140625" customWidth="1"/>
+    <col min="7" max="7" width="21.58203125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.58203125" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.08203125" customWidth="1"/>
+    <col min="12" max="12" width="18.58203125" customWidth="1"/>
+    <col min="13" max="13" width="13.08203125" customWidth="1"/>
     <col min="14" max="1025" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8657,7 +8671,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="18">
+    <row r="2" spans="1:8">
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="49.5" customHeight="1">
@@ -8671,7 +8685,7 @@
       <c r="F3" s="109"/>
       <c r="G3" s="109"/>
     </row>
-    <row r="4" spans="1:8" ht="18">
+    <row r="4" spans="1:8">
       <c r="C4" s="110" t="s">
         <v>3</v>
       </c>
@@ -8692,7 +8706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18">
+    <row r="7" spans="1:8">
       <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
@@ -8712,7 +8726,7 @@
       </c>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:8" ht="51.75">
+    <row r="9" spans="1:8" ht="52.2">
       <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
@@ -8726,7 +8740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="51.75">
+    <row r="10" spans="1:8" ht="52.2">
       <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
@@ -8737,7 +8751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="69">
+    <row r="11" spans="1:8" ht="69.599999999999994">
       <c r="C11" s="13" t="s">
         <v>20</v>
       </c>
@@ -8769,7 +8783,7 @@
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:8" ht="34.5">
+    <row r="15" spans="1:8" ht="34.799999999999997">
       <c r="C15" s="21" t="s">
         <v>26</v>
       </c>
@@ -8792,7 +8806,7 @@
       <c r="D19" s="111"/>
       <c r="E19" s="111"/>
     </row>
-    <row r="20" spans="3:5" ht="18">
+    <row r="20" spans="3:5">
       <c r="C20" s="24" t="s">
         <v>31</v>
       </c>
@@ -8800,7 +8814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="3:5" ht="18">
+    <row r="21" spans="3:5">
       <c r="C21" s="24" t="s">
         <v>33</v>
       </c>
@@ -8808,7 +8822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:5" ht="18">
+    <row r="22" spans="3:5">
       <c r="C22" s="24" t="s">
         <v>35</v>
       </c>
@@ -8816,7 +8830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:5" ht="18">
+    <row r="23" spans="3:5">
       <c r="C23" s="24" t="s">
         <v>37</v>
       </c>
@@ -8842,7 +8856,7 @@
       </c>
       <c r="E26" s="107"/>
     </row>
-    <row r="27" spans="3:5" ht="51.75">
+    <row r="27" spans="3:5" ht="52.2">
       <c r="C27" s="26" t="s">
         <v>43</v>
       </c>
@@ -8867,14 +8881,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y207"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="5" max="5" width="21.75" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -19164,16 +19178,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H292"/>
+  <dimension ref="A1:H293"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="G292" sqref="G292"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="E293" sqref="E293:G293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -22644,6 +22658,18 @@
       </c>
       <c r="G292" s="106" t="s">
         <v>1846</v>
+      </c>
+    </row>
+    <row r="293" spans="5:7">
+      <c r="E293" s="112" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F293" s="112" t="str">
+        <f>菜单SAAS版!E78</f>
+        <v>iam_menu-78</v>
+      </c>
+      <c r="G293" s="112" t="s">
+        <v>1848</v>
       </c>
     </row>
   </sheetData>
@@ -22656,15 +22682,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.75" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
+    <col min="8" max="8" width="14.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -28550,15 +28576,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y223"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="24.75" customWidth="1"/>
+    <col min="6" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -33688,7 +33714,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="55" t="s">

</xml_diff>

<commit_message>
【imp】add permisison  create api for create project
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-iam-menu-user-role-label.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-iam-menu-user-role-label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\hzero-iam\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B8AA3B-FE2E-42AB-B311-279B7569B8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EE66AF-A75D-4EE1-9432-5B75BEA55FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5881" uniqueCount="1850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5883" uniqueCount="1852">
   <si>
     <r>
       <rPr>
@@ -7423,12 +7423,18 @@
   <si>
     <t>iam_menu_permission-308</t>
   </si>
+  <si>
+    <t>hzero-iam.choerodon-project-user.create</t>
+  </si>
+  <si>
+    <t>iam_menu_permission-309</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="94">
+  <fonts count="95">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -8005,6 +8011,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -8144,7 +8157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8278,6 +8291,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8293,7 +8307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -8662,11 +8676,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" customHeight="1">
       <c r="A1" s="4"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -8675,21 +8689,21 @@
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="49.5" customHeight="1">
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="109" t="s">
+      <c r="D3" s="108"/>
+      <c r="E3" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="110"/>
+      <c r="D4" s="111"/>
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
@@ -8800,11 +8814,11 @@
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="111" t="s">
+      <c r="C19" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
     </row>
     <row r="20" spans="3:5">
       <c r="C20" s="24" t="s">
@@ -8842,19 +8856,19 @@
       <c r="C25" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="107" t="s">
+      <c r="D25" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="107"/>
+      <c r="E25" s="108"/>
     </row>
     <row r="26" spans="3:5" ht="14.25" customHeight="1">
       <c r="C26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="107" t="s">
+      <c r="D26" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="107"/>
+      <c r="E26" s="108"/>
     </row>
     <row r="27" spans="3:5" ht="52.2">
       <c r="C27" s="26" t="s">
@@ -19178,10 +19192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H293"/>
+  <dimension ref="A1:H294"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="E293" sqref="E293:G293"/>
+      <selection activeCell="E294" sqref="E294:G294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -22661,15 +22675,27 @@
       </c>
     </row>
     <row r="293" spans="5:7">
-      <c r="E293" s="112" t="s">
+      <c r="E293" s="107" t="s">
         <v>1849</v>
       </c>
-      <c r="F293" s="112" t="str">
+      <c r="F293" s="107" t="str">
         <f>菜单SAAS版!E78</f>
         <v>iam_menu-78</v>
       </c>
-      <c r="G293" s="112" t="s">
+      <c r="G293" s="107" t="s">
         <v>1848</v>
+      </c>
+    </row>
+    <row r="294" spans="5:7">
+      <c r="E294" s="113" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F294" s="113" t="str">
+        <f>菜单SAAS版!E78</f>
+        <v>iam_menu-78</v>
+      </c>
+      <c r="G294" s="113" t="s">
+        <v>1850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>